<commit_message>
reformatting stations in joint zones
</commit_message>
<xml_diff>
--- a/London stations.xlsx
+++ b/London stations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="12" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="492" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="11" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="950" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="London stations" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="616">
   <si>
     <t>Station</t>
   </si>
@@ -1835,6 +1835,21 @@
     <t>Worcester Park</t>
   </si>
   <si>
+    <t>½</t>
+  </si>
+  <si>
+    <t>¾</t>
+  </si>
+  <si>
+    <t>2/3</t>
+  </si>
+  <si>
+    <t>6/7</t>
+  </si>
+  <si>
+    <t>5/6</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
@@ -1847,18 +1862,12 @@
     <t>9</t>
   </si>
   <si>
-    <t>2/3</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>¾</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -1866,15 +1875,6 @@
   </si>
   <si>
     <t>6</t>
-  </si>
-  <si>
-    <t>½</t>
-  </si>
-  <si>
-    <t>5/6</t>
-  </si>
-  <si>
-    <t>6/7</t>
   </si>
 </sst>
 </file>
@@ -1884,10 +1884,10 @@
   <numFmts count="4">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="DD\-MMM" numFmtId="165"/>
-    <numFmt formatCode="DD/MM/YY" numFmtId="166"/>
-    <numFmt formatCode="@" numFmtId="167"/>
+    <numFmt formatCode="@" numFmtId="166"/>
+    <numFmt formatCode="DD/MM/YY" numFmtId="167"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -1911,9 +1911,14 @@
       <sz val="10"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
+      <b val="true"/>
+      <sz val="18"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -1968,7 +1973,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -2048,10 +2053,28 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1"/>
+              <a:t>Abbey Road Abbey Wood Acton Acton Central Acton Town Albany Park Aldgate Aldgate East Alexandra Palace All Saints Alperton Amersham Anerley Angel Angel Road Archway Arnos Grove Arsenal Baker Street Balham Bank Banstead Barbican Barking Barkingside Barnehurst Barnes Barnes Bridge Barons Court Battersea Park Bayswater Beckenham Hill Beckenham Junction Beckton Beckton Park Becontree Bellingham Belmont Belsize Park Belvedere Bermondsey Berrylands Bethnal Green Bethnal Green Rail Bexley Bexleyheath Bickley Birkbeck Blackfriars Blackheath Blackhorse Road Blackwall Bond Street Borough Boston Manor Bounds Green Bow Church Bow Road Bowes Park Brent Cross Brentford Brimsdown Brixton Brockley Bromley North Bromley South Bromley-by-Bow Brondesbury Brondesbury Park Bruce Grove Buckhurst Hill Burnt Oak Bush Hill Park Bushey Caledonian Road Caledonian Road and Barnsbury Cambridge Heath Camden Road Camden Town Canada Water Canary Wharf Canning Town Cannon Street Canonbury Canons Park Carpenders Park Carshalton Carshalton Beeches Castle Bar Park Catford Catford Bridge Chadwell Heath Chalfont and Latimer Chalk Farm Chancery Lane Charing Cross Charlton Cheam Chelsfield Chesham Chessington North Chessington South Chigwell Chislehurst Chiswick Chiswick Park Chorleywood City Thameslink Clapham Common Clapham High Street Clapham Junction Clapham North Clapham South Clapton Clock House Cobham and Stoke D'Abernon Cockfosters Colindale Colliers Wood Coulsdon South Covent Garden Crayford Crews Hill Crofton Park Crossharbour and London Arena Crouch Hill Croxley Crystal Palace Custom House Cutty Sark for Maritime Greenwich Cyprus Dagenham Dock Dagenham East Dagenham Heathway Dalston Junction Dalston Kingsland Dartford Debden Denmark Hill Deptford Deptford Bridge Devons Road Dollis Hill Drayton Green Drayton Park Ealing Broadway Ealing Common Earls Court Earlsfield East Acton East Croydon East Dulwich East Finchley East Ham East India East Putney Eastcote Eden Park Edgware Edgware Road (Bakerloo) Edgware Road (Circle/District/Hammersmith and City) Edmonton Green Elephant and Castle Elm Park Elmers End Elmstead Woods Elstree and Borehamwood Eltham Elverson Road Embankment Emerson Park Enfield Chase Enfield Lock Enfield Town Epping Epsom Downs Erith Essex Road Euston Euston Square Ewell East Ewell West Fairlop Falconwood Farringdon Feltham Fenchurch Street Finchley Central Finchley Road Finchley Road and Frognal Finsbury Park Forest Gate Forest Hill Fulham Broadway Fulwell Gallions Reach Gants Hill Gidea Park Gipsy Hill Gloucester Road Golders Green Goldhawk Road Goodge Street Goodmayes Gordon Hill Gospel Oak Grange Hill Grange Park Great Portland Street Green Park Greenford Greenwich Grove Park Gunnersbury Hackbridge Hackney Central Hackney Downs Hackney Wick Hadley Wood Haggerston Hainault Hammersmith (District) Hammersmith (Met.) Hampstead Hampstead Heath Hampton Hampton Court Hampton Wick Hanger Lane Hanwell Harlesden Harold Wood Harringay Harringay Green Lanes Harrow and Wealdstone Harrow-on-the-Hill Hatch End Hatton Cross Haydons Road Hayes Hayes and Harlington Headstone Lane Heathrow Terminal 4 Heathrow Terminal 5 Heathrow Terminals 1 2 3 Hendon Central Herne Hill Heron Quays High Barnet High Street Kensington Highams Park Highbury and Islington Highgate Hillingdon Hither Green Holborn Holland Park Holloway Road Homerton Honor Oak Park Hornchurch Hornsey Hounslow Hounslow Central Hounslow East Hounslow West Hoxton Hyde Park Corner Ickenham Ilford Imperial Wharf Island Gardens Isleworth Kenley Kennington Kensal Green Kensal Rise Kensington (Olympia) Kent House Kentish Town Kentish Town West Kenton Kew Bridge Kew Gardens Kidbrooke Kilburn Kilburn High Road Kilburn Park King George V King's Cross Kings Cross St. Pancras Kingsbury Kingston Knightsbridge Knockholt Ladbroke Grove Ladywell Lambeth North Lancaster Gate Langdon Park Latimer Road Lee Leicester Square Lewisham Leyton Leyton Midland Road Leytonstone Leytonstone High Road Limehouse Liverpool Street London Bridge London City Airport London Fields Loughborough Junction Loughton Lower Sydenham Maida Vale Malden Manor Manor House Manor Park Mansion House Marble Arch Maryland Marylebone Maze Hill Mile End Mill Hill Broadway Mill Hill East Mitcham Eastfields Mitcham Junction Monument Moor Park Moorgate Morden Morden South Mornington Crescent Mortlake Motspur Park Mottingham Mudchute Neasden New Barnet New Beckenham New Cross New Cross Gate New Eltham New Malden New Southgate Newbury Park Norbiton Norbury North Acton North Dulwich North Ealing North Greenwich North Harrow North Sheen North Wembley Northfields Northolt Northolt Park Northwick Park Northwood Northwood Hills Norwood Junction Notting Hill Gate Nunhead Oakleigh Park Oakwood Old Street Orpington Osterley Oval Oxford Circus Paddington Palmers Green Park Royal Parsons Green Peckham Rye Penge East Penge West Perivale Petts Wood Piccadilly Circus Pimlico Pinner Plaistow Plumstead Ponders End Pontoon Dock Poplar Preston Road Prince Regent Pudding Mill Lane Purley Purley Oaks Putney Putney Bridge Queens Park Queens Road Peckham Queensbury Queenstown Road Queensway Radlett Rainham Ravensbourne Ravenscourt Park Rayners Lane Raynes Park Rectory Road Redbridge Reedham Regents Park Richmond Rickmansworth Riddlesdown Roding Valley Romford Rotherhithe Royal Albert Royal Oak Royal Victoria Ruislip Ruislip Gardens Ruislip Manor Russell Square Sanderstead Selhurst Seven Kings Seven Sisters Shadwell Shepherds Bush Shepherds Bush Market Shoreditch High Street Shortlands Sidcup Silver Street Slade Green Sloane Square Smitham Snaresbrook South Acton South Bermondsey South Croydon South Ealing South Hampstead South Harrow South Kensington South Kenton South Merton South Quay South Ruislip South Tottenham South Wimbledon South Woodford Southall Southbury Southfields Southgate Southwark St Helier St James Street St Johns St Margarets St Mary Cray St Pancras St. James's Park St. Johns Wood St. Pauls Stamford Brook Stamford Hill Stanmore Star Lane Stepney Green Stockwell Stoke Newington Stonebridge Park Stoneleigh Stratford Stratford High Street Stratford International Strawberry Hill Streatham Streatham Common Streatham Hill Sudbury and Harrow Road Sudbury Hill Sudbury Hill Harrow Sudbury Town Sundridge Park Surbiton Surrey Quays Sutton Sutton Common Swiss Cottage Sydenham Sydenham Hill Syon Lane Teddington Temple Thames Ditton Theydon Bois Thornton Heath Tolworth Tooting Tooting Bec Tooting Broadway Tottenham Court Road Tottenham Hale Totteridge and Whetstone Tower Gateway Tower Hill Tufnell Park Tulse Hill Turkey Street Turnham Green Turnpike Lane Twickenham Upminster Upminster Bridge Upney Upper Holloway Upper Warlingham Upton Park Uxbridge Vauxhall Victoria Waddon Wallington Walthamstow Central Walthamstow Queens Road Wandsworth Common Wandsworth Road Wandsworth Town Wanstead Wanstead Park Wapping Warren Street Warwick Avenue Waterloo Watford Watford High Street Watford Junction Welling Wembley Central Wembley Park Wembley Stadium West Acton West Brompton West Croydon West Drayton West Dulwich West Ealing West Finchley West Ham West Hampstead West Hampstead Thameslink West Harrow West India Quay West Kensington West Norwood West Ruislip West Silvertown West Sutton West Wickham Westbourne Park Westcombe Park Westferry Westminster White City White Hart Lane Whitechapel Whitton Whyteleafe Whyteleafe South Willesden Green Willesden Junction Wimbledon Wimbledon Chase Wimbledon Park Winchmore Hill Wood Green Wood Lane Wood Street Woodford Woodgrange Park Woodmansterne Woodside Park Woolwich Arsenal Woolwich Dockyard Worcester Park</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -5641,11 +5664,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="83534532"/>
-        <c:axId val="55360421"/>
+        <c:axId val="2017948"/>
+        <c:axId val="46752765"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83534532"/>
+        <c:axId val="2017948"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5653,7 +5676,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55360421"/>
+        <c:crossAx val="46752765"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -5665,7 +5688,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55360421"/>
+        <c:axId val="46752765"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5683,7 +5706,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83534532"/>
+        <c:crossAx val="2017948"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -5706,10 +5729,28 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1"/>
+              <a:t>Baker Street Charing Cross Edgware Road (Bakerloo) Elephant and Castle Embankment Harlesden Harrow and Wealdstone Kensal Green Kenton Kilburn Park Lambeth North Maida Vale Marylebone North Wembley Oxford Circus Paddington Piccadilly Circus Queens Park Regents Park South Kenton Stonebridge Park Warwick Avenue Waterloo Wembley Central Willesden Junction</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -5903,11 +5944,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="50566732"/>
-        <c:axId val="88478756"/>
+        <c:axId val="71687267"/>
+        <c:axId val="82848710"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50566732"/>
+        <c:axId val="71687267"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5915,7 +5956,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88478756"/>
+        <c:crossAx val="82848710"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -5927,7 +5968,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88478756"/>
+        <c:axId val="82848710"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5945,7 +5986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50566732"/>
+        <c:crossAx val="71687267"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -5968,10 +6009,28 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1"/>
+              <a:t>Station</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -7635,11 +7694,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="47275202"/>
-        <c:axId val="89334931"/>
+        <c:axId val="93322925"/>
+        <c:axId val="4867283"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47275202"/>
+        <c:axId val="93322925"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7647,7 +7706,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89334931"/>
+        <c:crossAx val="4867283"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -7659,7 +7718,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89334931"/>
+        <c:axId val="4867283"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7677,7 +7736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47275202"/>
+        <c:crossAx val="93322925"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -7705,15 +7764,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>93600</xdr:colOff>
+      <xdr:colOff>120600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>172080</xdr:rowOff>
+      <xdr:rowOff>163080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>407520</xdr:colOff>
+      <xdr:colOff>434160</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7721,8 +7780,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3906720" y="172080"/>
-        <a:ext cx="17854560" cy="7276680"/>
+        <a:off x="3933720" y="163080"/>
+        <a:ext cx="17854200" cy="7276320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7740,15 +7799,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>465120</xdr:colOff>
+      <xdr:colOff>492120</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>77400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>140760</xdr:colOff>
+      <xdr:colOff>167400</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7756,8 +7815,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5803560" y="848160"/>
-        <a:ext cx="14165640" cy="3990960"/>
+        <a:off x="5830560" y="839160"/>
+        <a:ext cx="14165280" cy="3990600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7775,15 +7834,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>121680</xdr:colOff>
+      <xdr:colOff>148680</xdr:colOff>
       <xdr:row>218</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>216720</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>259</xdr:row>
-      <xdr:rowOff>144720</xdr:rowOff>
+      <xdr:rowOff>135360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7791,8 +7850,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9640080" y="38954160"/>
-        <a:ext cx="14585040" cy="7438680"/>
+        <a:off x="9667080" y="38945160"/>
+        <a:ext cx="14584680" cy="7438320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -20136,8 +20195,8 @@
   </sheetPr>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A24" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F59" activeCellId="0" pane="topLeft" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20301,8 +20360,8 @@
       <c r="E8" s="0" t="n">
         <v>-0.12416262739225</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <v>41367</v>
+      <c r="F8" s="1" t="s">
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
@@ -20402,7 +20461,7 @@
         <v>-0.19429940765557</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>14</v>
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
@@ -20505,7 +20564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>264</v>
       </c>
@@ -20521,8 +20580,8 @@
       <c r="E19" s="0" t="n">
         <v>-0.42336616986103</v>
       </c>
-      <c r="F19" s="0" t="s">
-        <v>265</v>
+      <c r="F19" s="2" t="s">
+        <v>606</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
@@ -20805,7 +20864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
         <v>341</v>
       </c>
@@ -20821,8 +20880,8 @@
       <c r="E34" s="0" t="n">
         <v>-0.095670549505162</v>
       </c>
-      <c r="F34" s="1" t="n">
-        <v>41335</v>
+      <c r="F34" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
@@ -21224,7 +21283,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="F14" activeCellId="0" pane="topLeft" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21489,7 +21548,7 @@
         <v>-0.12381555294752</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>14</v>
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
@@ -21570,8 +21629,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D42" activeCellId="0" pane="topLeft" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21657,15 +21716,15 @@
   </sheetPr>
   <dimension ref="A1:G271"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A228" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F273" activeCellId="0" pane="topLeft" sqref="F273"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A242" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2793522267206"/>
     <col collapsed="false" hidden="false" max="6" min="2" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
@@ -21706,8 +21765,8 @@
       <c r="E2" s="0" t="n">
         <v>-0.2802882961706</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>602</v>
+      <c r="F2" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
@@ -21726,8 +21785,8 @@
       <c r="E3" s="0" t="n">
         <v>-0.075612503707184</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>603</v>
+      <c r="F3" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="4">
@@ -21746,8 +21805,8 @@
       <c r="E4" s="0" t="n">
         <v>-0.072987053548915</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>603</v>
+      <c r="F4" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="5">
@@ -21766,8 +21825,8 @@
       <c r="E5" s="0" t="n">
         <v>-0.2995013414547</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>604</v>
+      <c r="F5" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
@@ -21786,8 +21845,8 @@
       <c r="E6" s="0" t="n">
         <v>-0.60649933056891</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>605</v>
+      <c r="F6" s="2" t="s">
+        <v>610</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
@@ -21806,8 +21865,8 @@
       <c r="E7" s="0" t="n">
         <v>-0.10556703413728</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>603</v>
+      <c r="F7" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
@@ -21826,8 +21885,8 @@
       <c r="E8" s="0" t="n">
         <v>-0.13510715160572</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>606</v>
+      <c r="F8" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="9">
@@ -21846,8 +21905,8 @@
       <c r="E9" s="0" t="n">
         <v>-0.13425577761924</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>604</v>
+      <c r="F9" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
@@ -21866,8 +21925,8 @@
       <c r="E10" s="0" t="n">
         <v>-0.10548551071377</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>607</v>
+      <c r="F10" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
@@ -21886,8 +21945,8 @@
       <c r="E11" s="0" t="n">
         <v>-0.15688978273689</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>603</v>
+      <c r="F11" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="12">
@@ -21906,8 +21965,8 @@
       <c r="E12" s="0" t="n">
         <v>-0.15267077683302</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>602</v>
+      <c r="F12" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
@@ -21926,8 +21985,8 @@
       <c r="E13" s="0" t="n">
         <v>-0.088985715325045</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>603</v>
+      <c r="F13" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="14">
@@ -21946,8 +22005,8 @@
       <c r="E14" s="0" t="n">
         <v>-0.097707167852645</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>603</v>
+      <c r="F14" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
@@ -21966,8 +22025,8 @@
       <c r="E15" s="0" t="n">
         <v>0.0808460268962</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>604</v>
+      <c r="F15" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16">
@@ -21986,8 +22045,8 @@
       <c r="E16" s="0" t="n">
         <v>0.088491071171579</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>604</v>
+      <c r="F16" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
@@ -22006,8 +22065,8 @@
       <c r="E17" s="0" t="n">
         <v>-0.21341574380466</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>607</v>
+      <c r="F17" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="18">
@@ -22026,8 +22085,8 @@
       <c r="E18" s="0" t="n">
         <v>-0.18788716574986</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>603</v>
+      <c r="F18" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="19">
@@ -22046,8 +22105,8 @@
       <c r="E19" s="0" t="n">
         <v>0.12689470862039</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>608</v>
+      <c r="F19" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
@@ -22066,8 +22125,8 @@
       <c r="E20" s="0" t="n">
         <v>-0.1639600723677</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>607</v>
+      <c r="F20" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="21">
@@ -22086,8 +22145,8 @@
       <c r="E21" s="0" t="n">
         <v>-0.064315686265478</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>607</v>
+      <c r="F21" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="22">
@@ -22106,8 +22165,8 @@
       <c r="E22" s="0" t="n">
         <v>-0.055377698622437</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>607</v>
+      <c r="F22" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="23">
@@ -22126,8 +22185,8 @@
       <c r="E23" s="0" t="n">
         <v>-0.10298097717171</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>603</v>
+      <c r="F23" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="24">
@@ -22146,8 +22205,8 @@
       <c r="E24" s="0" t="n">
         <v>-0.039611280026926</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>602</v>
+      <c r="F24" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="25">
@@ -22166,8 +22225,8 @@
       <c r="E25" s="0" t="n">
         <v>-0.14959920109132</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>603</v>
+      <c r="F25" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
@@ -22186,8 +22245,8 @@
       <c r="E26" s="0" t="n">
         <v>-0.094182918403389</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>603</v>
+      <c r="F26" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
@@ -22206,8 +22265,8 @@
       <c r="E27" s="0" t="n">
         <v>-0.32473278589022</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>604</v>
+      <c r="F27" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
@@ -22226,11 +22285,11 @@
       <c r="E28" s="0" t="n">
         <v>-0.12416262739225</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>609</v>
+      <c r="F28" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
@@ -22249,8 +22308,8 @@
       <c r="E29" s="0" t="n">
         <v>-0.020485486059214</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>607</v>
+      <c r="F29" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
@@ -22269,8 +22328,8 @@
       <c r="E30" s="0" t="n">
         <v>-0.024345177705763</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>607</v>
+      <c r="F30" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="31">
@@ -22289,8 +22348,8 @@
       <c r="E31" s="0" t="n">
         <v>-0.21332141198154</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>602</v>
+      <c r="F31" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="32">
@@ -22309,8 +22368,8 @@
       <c r="E32" s="0" t="n">
         <v>-0.11453770490964</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>607</v>
+      <c r="F32" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
@@ -22329,11 +22388,11 @@
       <c r="E33" s="0" t="n">
         <v>-0.01166796209473</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>606</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>606</v>
+      <c r="F33" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="34">
@@ -22352,8 +22411,8 @@
       <c r="E34" s="0" t="n">
         <v>0.046726985755</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>608</v>
+      <c r="F34" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="35">
@@ -22372,8 +22431,8 @@
       <c r="E35" s="0" t="n">
         <v>-0.26431627556888</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>604</v>
+      <c r="F35" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="36">
@@ -22392,8 +22451,8 @@
       <c r="E36" s="0" t="n">
         <v>-0.11834644235876</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>607</v>
+      <c r="F36" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="37">
@@ -22412,8 +22471,8 @@
       <c r="E37" s="0" t="n">
         <v>-0.14243796405007</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>607</v>
+      <c r="F37" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="38">
@@ -22432,8 +22491,8 @@
       <c r="E38" s="0" t="n">
         <v>-0.05079271714472</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>607</v>
+      <c r="F38" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39">
@@ -22452,8 +22511,8 @@
       <c r="E39" s="0" t="n">
         <v>-0.019452434600173</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>607</v>
+      <c r="F39" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="40">
@@ -22472,8 +22531,8 @@
       <c r="E40" s="0" t="n">
         <v>0.0083200415480822</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>602</v>
+      <c r="F40" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="41">
@@ -22492,8 +22551,8 @@
       <c r="E41" s="0" t="n">
         <v>-0.090236118885105</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>603</v>
+      <c r="F41" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="42">
@@ -22512,8 +22571,8 @@
       <c r="E42" s="0" t="n">
         <v>-0.29437715826231</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>608</v>
+      <c r="F42" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="43">
@@ -22532,8 +22591,8 @@
       <c r="E43" s="0" t="n">
         <v>-0.56105332039672</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>610</v>
+      <c r="F43" s="2" t="s">
+        <v>613</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="44">
@@ -22552,8 +22611,8 @@
       <c r="E44" s="0" t="n">
         <v>-0.15371865256093</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>607</v>
+      <c r="F44" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="45">
@@ -22572,8 +22631,8 @@
       <c r="E45" s="0" t="n">
         <v>-0.11194761724718</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>603</v>
+      <c r="F45" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="46">
@@ -22592,8 +22651,8 @@
       <c r="E46" s="0" t="n">
         <v>-0.12478853109718</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>603</v>
+      <c r="F46" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="47">
@@ -22612,8 +22671,8 @@
       <c r="E47" s="0" t="n">
         <v>-0.61141518839627</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>605</v>
+      <c r="F47" s="2" t="s">
+        <v>610</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="48">
@@ -22632,8 +22691,8 @@
       <c r="E48" s="0" t="n">
         <v>0.076193656688014</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>604</v>
+      <c r="F48" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="49">
@@ -22652,8 +22711,8 @@
       <c r="E49" s="0" t="n">
         <v>-0.26772251965492</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>602</v>
+      <c r="F49" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="50">
@@ -22672,8 +22731,8 @@
       <c r="E50" s="0" t="n">
         <v>-0.51831947385278</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>611</v>
+      <c r="F50" s="2" t="s">
+        <v>614</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="51">
@@ -22692,8 +22751,8 @@
       <c r="E51" s="0" t="n">
         <v>-0.13830051012379</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>607</v>
+      <c r="F51" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="52">
@@ -22712,8 +22771,8 @@
       <c r="E52" s="0" t="n">
         <v>-0.12989566953588</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>607</v>
+      <c r="F52" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="53">
@@ -22732,11 +22791,11 @@
       <c r="E53" s="0" t="n">
         <v>-0.1479696801021</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>606</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>606</v>
+      <c r="F53" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="54">
@@ -22755,8 +22814,8 @@
       <c r="E54" s="0" t="n">
         <v>-0.14990225857042</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>608</v>
+      <c r="F54" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="55">
@@ -22775,8 +22834,8 @@
       <c r="E55" s="0" t="n">
         <v>-0.25027310932225</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>604</v>
+      <c r="F55" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="56">
@@ -22795,8 +22854,8 @@
       <c r="E56" s="0" t="n">
         <v>-0.17740072104762</v>
       </c>
-      <c r="F56" s="3" t="s">
-        <v>602</v>
+      <c r="F56" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="57">
@@ -22815,8 +22874,8 @@
       <c r="E57" s="0" t="n">
         <v>-0.1244924862088</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>603</v>
+      <c r="F57" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="58">
@@ -22835,8 +22894,8 @@
       <c r="E58" s="0" t="n">
         <v>-0.44158934771671</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>611</v>
+      <c r="F58" s="2" t="s">
+        <v>614</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="59">
@@ -22855,8 +22914,8 @@
       <c r="E59" s="0" t="n">
         <v>0.16584784999223</v>
       </c>
-      <c r="F59" s="3" t="s">
-        <v>608</v>
+      <c r="F59" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="60">
@@ -22875,8 +22934,8 @@
       <c r="E60" s="0" t="n">
         <v>0.14769413756505</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>608</v>
+      <c r="F60" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="61">
@@ -22895,8 +22954,8 @@
       <c r="E61" s="0" t="n">
         <v>0.083815925291538</v>
       </c>
-      <c r="F61" s="3" t="s">
-        <v>612</v>
+      <c r="F61" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="62">
@@ -22915,8 +22974,8 @@
       <c r="E62" s="0" t="n">
         <v>-0.23878334100376</v>
       </c>
-      <c r="F62" s="3" t="s">
-        <v>602</v>
+      <c r="F62" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="63">
@@ -22935,8 +22994,8 @@
       <c r="E63" s="0" t="n">
         <v>-0.30199597251937</v>
       </c>
-      <c r="F63" s="3" t="s">
-        <v>602</v>
+      <c r="F63" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="64">
@@ -22955,8 +23014,8 @@
       <c r="E64" s="0" t="n">
         <v>-0.28713701041592</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>602</v>
+      <c r="F64" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="65">
@@ -22975,11 +23034,11 @@
       <c r="E65" s="0" t="n">
         <v>-0.19429940765557</v>
       </c>
-      <c r="F65" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>613</v>
+      <c r="F65" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="66">
@@ -22998,8 +23057,8 @@
       <c r="E66" s="0" t="n">
         <v>-0.2480978154307</v>
       </c>
-      <c r="F66" s="3" t="s">
-        <v>607</v>
+      <c r="F66" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="67">
@@ -23018,8 +23077,8 @@
       <c r="E67" s="0" t="n">
         <v>-0.16472945405368</v>
       </c>
-      <c r="F67" s="3" t="s">
-        <v>602</v>
+      <c r="F67" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="68">
@@ -23038,11 +23097,11 @@
       <c r="E68" s="0" t="n">
         <v>0.051530710126145</v>
       </c>
-      <c r="F68" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>609</v>
+      <c r="F68" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="69">
@@ -23061,11 +23120,11 @@
       <c r="E69" s="0" t="n">
         <v>-0.21098384278422</v>
       </c>
-      <c r="F69" s="3" t="s">
-        <v>606</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>606</v>
+      <c r="F69" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="70">
@@ -23084,8 +23143,8 @@
       <c r="E70" s="0" t="n">
         <v>-0.39680887105797</v>
       </c>
-      <c r="F70" s="3" t="s">
-        <v>608</v>
+      <c r="F70" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="71">
@@ -23104,8 +23163,8 @@
       <c r="E71" s="0" t="n">
         <v>-0.27507922607818</v>
       </c>
-      <c r="F71" s="3" t="s">
-        <v>608</v>
+      <c r="F71" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="72">
@@ -23124,8 +23183,8 @@
       <c r="E72" s="0" t="n">
         <v>-0.17052514070378</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>603</v>
+      <c r="F72" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="73">
@@ -23144,8 +23203,8 @@
       <c r="E73" s="0" t="n">
         <v>-0.1676538436008</v>
       </c>
-      <c r="F73" s="3" t="s">
-        <v>603</v>
+      <c r="F73" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="74">
@@ -23164,11 +23223,11 @@
       <c r="E74" s="0" t="n">
         <v>-0.10072431173602</v>
       </c>
-      <c r="F74" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>613</v>
+      <c r="F74" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="75">
@@ -23187,8 +23246,8 @@
       <c r="E75" s="0" t="n">
         <v>0.19726710182967</v>
       </c>
-      <c r="F75" s="3" t="s">
-        <v>612</v>
+      <c r="F75" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="76">
@@ -23207,8 +23266,8 @@
       <c r="E76" s="0" t="n">
         <v>-0.12235292981979</v>
       </c>
-      <c r="F76" s="3" t="s">
-        <v>603</v>
+      <c r="F76" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="77">
@@ -23227,8 +23286,8 @@
       <c r="E77" s="0" t="n">
         <v>0.11384001852178</v>
       </c>
-      <c r="F77" s="3" t="s">
-        <v>612</v>
+      <c r="F77" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="78">
@@ -23247,8 +23306,8 @@
       <c r="E78" s="0" t="n">
         <v>-0.13328205840994</v>
       </c>
-      <c r="F78" s="3" t="s">
-        <v>603</v>
+      <c r="F78" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="79">
@@ -23267,8 +23326,8 @@
       <c r="E79" s="0" t="n">
         <v>-0.13328205840994</v>
       </c>
-      <c r="F79" s="3" t="s">
-        <v>603</v>
+      <c r="F79" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="80">
@@ -23287,8 +23346,8 @@
       <c r="E80" s="0" t="n">
         <v>0.090607714208087</v>
       </c>
-      <c r="F80" s="3" t="s">
-        <v>604</v>
+      <c r="F80" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="81">
@@ -23307,8 +23366,8 @@
       <c r="E81" s="0" t="n">
         <v>-0.10482865117184</v>
       </c>
-      <c r="F81" s="3" t="s">
-        <v>603</v>
+      <c r="F81" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="82">
@@ -23327,8 +23386,8 @@
       <c r="E82" s="0" t="n">
         <v>-0.19320620063466</v>
       </c>
-      <c r="F82" s="3" t="s">
-        <v>604</v>
+      <c r="F82" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="83">
@@ -23347,8 +23406,8 @@
       <c r="E83" s="0" t="n">
         <v>-0.18003614128656</v>
       </c>
-      <c r="F83" s="3" t="s">
-        <v>607</v>
+      <c r="F83" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="84">
@@ -23367,8 +23426,8 @@
       <c r="E84" s="0" t="n">
         <v>-0.10586706135916</v>
       </c>
-      <c r="F84" s="3" t="s">
-        <v>607</v>
+      <c r="F84" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="85">
@@ -23387,8 +23446,8 @@
       <c r="E85" s="0" t="n">
         <v>-0.19552976561085</v>
       </c>
-      <c r="F85" s="3" t="s">
-        <v>607</v>
+      <c r="F85" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="86">
@@ -23407,8 +23466,8 @@
       <c r="E86" s="0" t="n">
         <v>0.066098526398209</v>
       </c>
-      <c r="F86" s="3" t="s">
-        <v>604</v>
+      <c r="F86" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="87">
@@ -23427,8 +23486,8 @@
       <c r="E87" s="0" t="n">
         <v>-0.18352915689619</v>
       </c>
-      <c r="F87" s="3" t="s">
-        <v>603</v>
+      <c r="F87" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="88">
@@ -23447,8 +23506,8 @@
       <c r="E88" s="0" t="n">
         <v>-0.19482013198437</v>
       </c>
-      <c r="F88" s="3" t="s">
-        <v>602</v>
+      <c r="F88" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="89">
@@ -23467,8 +23526,8 @@
       <c r="E89" s="0" t="n">
         <v>-0.22738960127533</v>
       </c>
-      <c r="F89" s="3" t="s">
-        <v>607</v>
+      <c r="F89" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="90">
@@ -23487,8 +23546,8 @@
       <c r="E90" s="0" t="n">
         <v>-0.13479327927061</v>
       </c>
-      <c r="F90" s="3" t="s">
-        <v>603</v>
+      <c r="F90" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="91">
@@ -23507,8 +23566,8 @@
       <c r="E91" s="0" t="n">
         <v>0.092286969949084</v>
       </c>
-      <c r="F91" s="3" t="s">
-        <v>604</v>
+      <c r="F91" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="92">
@@ -23527,8 +23586,8 @@
       <c r="E92" s="0" t="n">
         <v>-0.14394701338886</v>
       </c>
-      <c r="F92" s="3" t="s">
-        <v>603</v>
+      <c r="F92" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="93">
@@ -23547,8 +23606,8 @@
       <c r="E93" s="0" t="n">
         <v>-0.14246316907526</v>
       </c>
-      <c r="F93" s="3" t="s">
-        <v>603</v>
+      <c r="F93" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="94">
@@ -23567,8 +23626,8 @@
       <c r="E94" s="0" t="n">
         <v>-0.34586432267848</v>
       </c>
-      <c r="F94" s="3" t="s">
-        <v>604</v>
+      <c r="F94" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="95">
@@ -23587,8 +23646,8 @@
       <c r="E95" s="0" t="n">
         <v>-0.27514973411264</v>
       </c>
-      <c r="F95" s="3" t="s">
-        <v>602</v>
+      <c r="F95" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="96">
@@ -23607,8 +23666,8 @@
       <c r="E96" s="0" t="n">
         <v>0.094122987217226</v>
       </c>
-      <c r="F96" s="3" t="s">
-        <v>604</v>
+      <c r="F96" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="97">
@@ -23627,8 +23686,8 @@
       <c r="E97" s="0" t="n">
         <v>-0.22284652701972</v>
       </c>
-      <c r="F97" s="3" t="s">
-        <v>607</v>
+      <c r="F97" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="98">
@@ -23647,8 +23706,8 @@
       <c r="E98" s="0" t="n">
         <v>-0.22462575515926</v>
       </c>
-      <c r="F98" s="3" t="s">
-        <v>607</v>
+      <c r="F98" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="99">
@@ -23667,8 +23726,8 @@
       <c r="E99" s="0" t="n">
         <v>-0.17800013773286</v>
       </c>
-      <c r="F99" s="3" t="s">
-        <v>607</v>
+      <c r="F99" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="100">
@@ -23687,8 +23746,8 @@
       <c r="E100" s="0" t="n">
         <v>-0.29298173181915</v>
       </c>
-      <c r="F100" s="3" t="s">
-        <v>602</v>
+      <c r="F100" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="101">
@@ -23707,8 +23766,8 @@
       <c r="E101" s="0" t="n">
         <v>-0.25748125850322</v>
       </c>
-      <c r="F101" s="3" t="s">
-        <v>602</v>
+      <c r="F101" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="102">
@@ -23727,8 +23786,8 @@
       <c r="E102" s="0" t="n">
         <v>-0.33423825163137</v>
       </c>
-      <c r="F102" s="3" t="s">
-        <v>608</v>
+      <c r="F102" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="103">
@@ -23747,8 +23806,8 @@
       <c r="E103" s="0" t="n">
         <v>-0.33698708805734</v>
       </c>
-      <c r="F103" s="3" t="s">
-        <v>608</v>
+      <c r="F103" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="104">
@@ -23767,11 +23826,11 @@
       <c r="E104" s="0" t="n">
         <v>-0.42336616986103</v>
       </c>
-      <c r="F104" s="3" t="s">
-        <v>614</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>614</v>
+      <c r="F104" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>606</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="105">
@@ -23790,8 +23849,8 @@
       <c r="E105" s="0" t="n">
         <v>-0.44771519861354</v>
       </c>
-      <c r="F105" s="3" t="s">
-        <v>612</v>
+      <c r="F105" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="106">
@@ -23810,8 +23869,8 @@
       <c r="E106" s="0" t="n">
         <v>-0.49063310869077</v>
       </c>
-      <c r="F106" s="3" t="s">
-        <v>612</v>
+      <c r="F106" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="107">
@@ -23830,8 +23889,8 @@
       <c r="E107" s="0" t="n">
         <v>-0.45239283063262</v>
       </c>
-      <c r="F107" s="3" t="s">
-        <v>612</v>
+      <c r="F107" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="108">
@@ -23850,11 +23909,11 @@
       <c r="E108" s="0" t="n">
         <v>-0.2267197095034</v>
       </c>
-      <c r="F108" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>609</v>
+      <c r="F108" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="109">
@@ -23873,8 +23932,8 @@
       <c r="E109" s="0" t="n">
         <v>-0.19415092780429</v>
       </c>
-      <c r="F109" s="3" t="s">
-        <v>608</v>
+      <c r="F109" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="110">
@@ -23893,8 +23952,8 @@
       <c r="E110" s="0" t="n">
         <v>-0.19155165303998</v>
       </c>
-      <c r="F110" s="3" t="s">
-        <v>603</v>
+      <c r="F110" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="111">
@@ -23913,8 +23972,8 @@
       <c r="E111" s="0" t="n">
         <v>-0.10406772078143</v>
       </c>
-      <c r="F111" s="3" t="s">
-        <v>607</v>
+      <c r="F111" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="112">
@@ -23933,8 +23992,8 @@
       <c r="E112" s="0" t="n">
         <v>-0.14692043327249</v>
       </c>
-      <c r="F112" s="3" t="s">
-        <v>602</v>
+      <c r="F112" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="113">
@@ -23953,8 +24012,8 @@
       <c r="E113" s="0" t="n">
         <v>-0.44988357245777</v>
       </c>
-      <c r="F113" s="3" t="s">
-        <v>612</v>
+      <c r="F113" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="114">
@@ -23973,8 +24032,8 @@
       <c r="E114" s="0" t="n">
         <v>-0.11982609759457</v>
       </c>
-      <c r="F114" s="3" t="s">
-        <v>603</v>
+      <c r="F114" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="115">
@@ -23993,8 +24052,8 @@
       <c r="E115" s="0" t="n">
         <v>-0.20654337129402</v>
       </c>
-      <c r="F115" s="3" t="s">
-        <v>607</v>
+      <c r="F115" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="116">
@@ -24013,8 +24072,8 @@
       <c r="E116" s="0" t="n">
         <v>-0.11292127587712</v>
       </c>
-      <c r="F116" s="3" t="s">
-        <v>607</v>
+      <c r="F116" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="117">
@@ -24033,8 +24092,8 @@
       <c r="E117" s="0" t="n">
         <v>0.21894141805997</v>
       </c>
-      <c r="F117" s="3" t="s">
-        <v>612</v>
+      <c r="F117" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="118">
@@ -24053,8 +24112,8 @@
       <c r="E118" s="0" t="n">
         <v>-0.36594373417825</v>
       </c>
-      <c r="F118" s="3" t="s">
-        <v>604</v>
+      <c r="F118" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="119">
@@ -24073,8 +24132,8 @@
       <c r="E119" s="0" t="n">
         <v>-0.35526092596841</v>
       </c>
-      <c r="F119" s="3" t="s">
-        <v>604</v>
+      <c r="F119" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="120">
@@ -24093,8 +24152,8 @@
       <c r="E120" s="0" t="n">
         <v>-0.38569323300198</v>
       </c>
-      <c r="F120" s="3" t="s">
-        <v>608</v>
+      <c r="F120" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="121">
@@ -24113,8 +24172,8 @@
       <c r="E121" s="0" t="n">
         <v>-0.15245970877887</v>
       </c>
-      <c r="F121" s="3" t="s">
-        <v>603</v>
+      <c r="F121" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="122">
@@ -24133,8 +24192,8 @@
       <c r="E122" s="0" t="n">
         <v>-0.44156508942605</v>
       </c>
-      <c r="F122" s="3" t="s">
-        <v>612</v>
+      <c r="F122" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="123">
@@ -24153,8 +24212,8 @@
       <c r="E123" s="0" t="n">
         <v>-0.10505621257104</v>
       </c>
-      <c r="F123" s="3" t="s">
-        <v>607</v>
+      <c r="F123" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="124">
@@ -24173,8 +24232,8 @@
       <c r="E124" s="0" t="n">
         <v>-0.22469897011847</v>
       </c>
-      <c r="F124" s="3" t="s">
-        <v>607</v>
+      <c r="F124" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="125">
@@ -24193,8 +24252,8 @@
       <c r="E125" s="0" t="n">
         <v>-0.21036483866639</v>
       </c>
-      <c r="F125" s="3" t="s">
-        <v>607</v>
+      <c r="F125" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="126">
@@ -24213,8 +24272,8 @@
       <c r="E126" s="0" t="n">
         <v>-0.14045684366827</v>
       </c>
-      <c r="F126" s="3" t="s">
-        <v>607</v>
+      <c r="F126" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="127">
@@ -24233,8 +24292,8 @@
       <c r="E127" s="0" t="n">
         <v>-0.31520243664979</v>
       </c>
-      <c r="F127" s="3" t="s">
-        <v>604</v>
+      <c r="F127" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="128">
@@ -24253,11 +24312,11 @@
       <c r="E128" s="0" t="n">
         <v>-0.28536661446493</v>
       </c>
-      <c r="F128" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="G128" s="3" t="s">
-        <v>609</v>
+      <c r="F128" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="129">
@@ -24276,8 +24335,8 @@
       <c r="E129" s="0" t="n">
         <v>-0.20461829997264</v>
       </c>
-      <c r="F129" s="3" t="s">
-        <v>607</v>
+      <c r="F129" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="130">
@@ -24296,8 +24355,8 @@
       <c r="E130" s="0" t="n">
         <v>-0.19395164168612</v>
       </c>
-      <c r="F130" s="3" t="s">
-        <v>607</v>
+      <c r="F130" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="131">
@@ -24316,8 +24375,8 @@
       <c r="E131" s="0" t="n">
         <v>-0.12385771561154</v>
       </c>
-      <c r="F131" s="3" t="s">
-        <v>603</v>
+      <c r="F131" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="132">
@@ -24336,8 +24395,8 @@
       <c r="E132" s="0" t="n">
         <v>-0.27858717715014</v>
       </c>
-      <c r="F132" s="3" t="s">
-        <v>604</v>
+      <c r="F132" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="133">
@@ -24356,8 +24415,8 @@
       <c r="E133" s="0" t="n">
         <v>-0.16065008131194</v>
       </c>
-      <c r="F133" s="3" t="s">
-        <v>603</v>
+      <c r="F133" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="134">
@@ -24376,8 +24435,8 @@
       <c r="E134" s="0" t="n">
         <v>-0.21018376269161</v>
       </c>
-      <c r="F134" s="3" t="s">
-        <v>607</v>
+      <c r="F134" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="135">
@@ -24396,8 +24455,8 @@
       <c r="E135" s="0" t="n">
         <v>-0.11175385704735</v>
       </c>
-      <c r="F135" s="3" t="s">
-        <v>603</v>
+      <c r="F135" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="136">
@@ -24416,8 +24475,8 @@
       <c r="E136" s="0" t="n">
         <v>-0.17541552045722</v>
       </c>
-      <c r="F136" s="3" t="s">
-        <v>603</v>
+      <c r="F136" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="137">
@@ -24436,8 +24495,8 @@
       <c r="E137" s="0" t="n">
         <v>-0.21744525733064</v>
       </c>
-      <c r="F137" s="3" t="s">
-        <v>607</v>
+      <c r="F137" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="138">
@@ -24456,8 +24515,8 @@
       <c r="E138" s="0" t="n">
         <v>-0.12822773962177</v>
       </c>
-      <c r="F138" s="3" t="s">
-        <v>603</v>
+      <c r="F138" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="139">
@@ -24476,8 +24535,8 @@
       <c r="E139" s="0" t="n">
         <v>-0.0064509088011814</v>
       </c>
-      <c r="F139" s="3" t="s">
-        <v>602</v>
+      <c r="F139" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="140">
@@ -24496,11 +24555,11 @@
       <c r="E140" s="0" t="n">
         <v>0.009154878018083</v>
       </c>
-      <c r="F140" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="G140" s="3" t="s">
-        <v>609</v>
+      <c r="F140" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="141">
@@ -24519,8 +24578,8 @@
       <c r="E141" s="0" t="n">
         <v>-0.082235212309326</v>
       </c>
-      <c r="F141" s="3" t="s">
-        <v>603</v>
+      <c r="F141" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="142">
@@ -24539,8 +24598,8 @@
       <c r="E142" s="0" t="n">
         <v>-0.085991192281661</v>
       </c>
-      <c r="F142" s="3" t="s">
-        <v>603</v>
+      <c r="F142" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="143">
@@ -24559,8 +24618,8 @@
       <c r="E143" s="0" t="n">
         <v>0.055293528321119</v>
       </c>
-      <c r="F143" s="3" t="s">
-        <v>612</v>
+      <c r="F143" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="144">
@@ -24579,8 +24638,8 @@
       <c r="E144" s="0" t="n">
         <v>-0.18541823310956</v>
       </c>
-      <c r="F144" s="3" t="s">
-        <v>607</v>
+      <c r="F144" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="145">
@@ -24599,11 +24658,11 @@
       <c r="E145" s="0" t="n">
         <v>-0.095670549505162</v>
       </c>
-      <c r="F145" s="3" t="s">
-        <v>606</v>
-      </c>
-      <c r="G145" s="3" t="s">
-        <v>606</v>
+      <c r="F145" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="146">
@@ -24622,8 +24681,8 @@
       <c r="E146" s="0" t="n">
         <v>-0.094183249527509</v>
       </c>
-      <c r="F146" s="3" t="s">
-        <v>603</v>
+      <c r="F146" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="147">
@@ -24642,8 +24701,8 @@
       <c r="E147" s="0" t="n">
         <v>-0.15855680746603</v>
       </c>
-      <c r="F147" s="3" t="s">
-        <v>603</v>
+      <c r="F147" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="148">
@@ -24662,8 +24721,8 @@
       <c r="E148" s="0" t="n">
         <v>-0.16347815242029</v>
       </c>
-      <c r="F148" s="3" t="s">
-        <v>603</v>
+      <c r="F148" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="149">
@@ -24682,8 +24741,8 @@
       <c r="E149" s="0" t="n">
         <v>-0.032651671918221</v>
       </c>
-      <c r="F149" s="3" t="s">
-        <v>607</v>
+      <c r="F149" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="150">
@@ -24702,8 +24761,8 @@
       <c r="E150" s="0" t="n">
         <v>-0.20988127429344</v>
       </c>
-      <c r="F150" s="3" t="s">
-        <v>604</v>
+      <c r="F150" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="151">
@@ -24722,8 +24781,8 @@
       <c r="E151" s="0" t="n">
         <v>-0.086173905918798</v>
       </c>
-      <c r="F151" s="3" t="s">
-        <v>603</v>
+      <c r="F151" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="152">
@@ -24742,11 +24801,11 @@
       <c r="E152" s="0" t="n">
         <v>-0.4328985822977</v>
       </c>
-      <c r="F152" s="3" t="s">
-        <v>615</v>
-      </c>
-      <c r="G152" s="3" t="s">
-        <v>615</v>
+      <c r="F152" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>605</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="153">
@@ -24765,8 +24824,8 @@
       <c r="E153" s="0" t="n">
         <v>-0.08900327764505</v>
       </c>
-      <c r="F153" s="3" t="s">
-        <v>603</v>
+      <c r="F153" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="154">
@@ -24785,8 +24844,8 @@
       <c r="E154" s="0" t="n">
         <v>-0.19483760810466</v>
       </c>
-      <c r="F154" s="3" t="s">
-        <v>604</v>
+      <c r="F154" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="155">
@@ -24805,8 +24864,8 @@
       <c r="E155" s="0" t="n">
         <v>-0.1387299346061</v>
       </c>
-      <c r="F155" s="3" t="s">
-        <v>607</v>
+      <c r="F155" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="156">
@@ -24825,8 +24884,8 @@
       <c r="E156" s="0" t="n">
         <v>-0.25010062378951</v>
       </c>
-      <c r="F156" s="3" t="s">
-        <v>602</v>
+      <c r="F156" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="157">
@@ -24845,8 +24904,8 @@
       <c r="E157" s="0" t="n">
         <v>0.090317586010402</v>
       </c>
-      <c r="F157" s="3" t="s">
-        <v>604</v>
+      <c r="F157" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="158">
@@ -24865,11 +24924,11 @@
       <c r="E158" s="0" t="n">
         <v>-0.25971511616691</v>
       </c>
-      <c r="F158" s="3" t="s">
-        <v>606</v>
-      </c>
-      <c r="G158" s="3" t="s">
-        <v>606</v>
+      <c r="F158" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="G158" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="159">
@@ -24888,8 +24947,8 @@
       <c r="E159" s="0" t="n">
         <v>-0.28897914280262</v>
       </c>
-      <c r="F159" s="3" t="s">
-        <v>602</v>
+      <c r="F159" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="160">
@@ -24908,8 +24967,8 @@
       <c r="E160" s="0" t="n">
         <v>0.0036006636371896</v>
       </c>
-      <c r="F160" s="3" t="s">
-        <v>606</v>
+      <c r="F160" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="161">
@@ -24928,8 +24987,8 @@
       <c r="E161" s="0" t="n">
         <v>-0.3626185623764</v>
       </c>
-      <c r="F161" s="3" t="s">
-        <v>608</v>
+      <c r="F161" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="162">
@@ -24948,8 +25007,8 @@
       <c r="E162" s="0" t="n">
         <v>-0.30393379535805</v>
       </c>
-      <c r="F162" s="3" t="s">
-        <v>604</v>
+      <c r="F162" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="163">
@@ -24968,8 +25027,8 @@
       <c r="E163" s="0" t="n">
         <v>-0.31505041439224</v>
       </c>
-      <c r="F163" s="3" t="s">
-        <v>602</v>
+      <c r="F163" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="164">
@@ -24988,8 +25047,8 @@
       <c r="E164" s="0" t="n">
         <v>-0.36842617615208</v>
       </c>
-      <c r="F164" s="3" t="s">
-        <v>608</v>
+      <c r="F164" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="165">
@@ -25008,8 +25067,8 @@
       <c r="E165" s="0" t="n">
         <v>-0.31818496289702</v>
       </c>
-      <c r="F165" s="3" t="s">
-        <v>604</v>
+      <c r="F165" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="166">
@@ -25028,8 +25087,8 @@
       <c r="E166" s="0" t="n">
         <v>-0.40929692189409</v>
       </c>
-      <c r="F166" s="3" t="s">
-        <v>612</v>
+      <c r="F166" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="167">
@@ -25048,11 +25107,11 @@
       <c r="E167" s="0" t="n">
         <v>-0.1959072111467</v>
       </c>
-      <c r="F167" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="G167" s="3" t="s">
-        <v>613</v>
+      <c r="F167" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="G167" s="2" t="s">
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="168">
@@ -25071,8 +25130,8 @@
       <c r="E168" s="0" t="n">
         <v>-0.1318390886991</v>
       </c>
-      <c r="F168" s="3" t="s">
-        <v>608</v>
+      <c r="F168" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="169">
@@ -25091,8 +25150,8 @@
       <c r="E169" s="0" t="n">
         <v>-0.087608545343845</v>
       </c>
-      <c r="F169" s="3" t="s">
-        <v>603</v>
+      <c r="F169" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="170">
@@ -25111,8 +25170,8 @@
       <c r="E170" s="0" t="n">
         <v>-0.3520816978192</v>
       </c>
-      <c r="F170" s="3" t="s">
-        <v>604</v>
+      <c r="F170" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="171">
@@ -25131,8 +25190,8 @@
       <c r="E171" s="0" t="n">
         <v>-0.11330667730935</v>
       </c>
-      <c r="F171" s="3" t="s">
-        <v>607</v>
+      <c r="F171" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="172">
@@ -25151,8 +25210,8 @@
       <c r="E172" s="0" t="n">
         <v>-0.14082176208955</v>
       </c>
-      <c r="F172" s="3" t="s">
-        <v>603</v>
+      <c r="F172" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="173">
@@ -25171,8 +25230,8 @@
       <c r="E173" s="0" t="n">
         <v>-0.17572234283505</v>
       </c>
-      <c r="F173" s="3" t="s">
-        <v>603</v>
+      <c r="F173" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="174">
@@ -25191,8 +25250,8 @@
       <c r="E174" s="0" t="n">
         <v>-0.17572234283505</v>
       </c>
-      <c r="F174" s="3" t="s">
-        <v>603</v>
+      <c r="F174" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="175">
@@ -25211,8 +25270,8 @@
       <c r="E175" s="0" t="n">
         <v>-0.28491450496891</v>
       </c>
-      <c r="F175" s="3" t="s">
-        <v>602</v>
+      <c r="F175" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="176">
@@ -25231,8 +25290,8 @@
       <c r="E176" s="0" t="n">
         <v>-0.20111009589714</v>
       </c>
-      <c r="F176" s="3" t="s">
-        <v>607</v>
+      <c r="F176" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="177">
@@ -25251,8 +25310,8 @@
       <c r="E177" s="0" t="n">
         <v>-0.32305600630537</v>
       </c>
-      <c r="F177" s="3" t="s">
-        <v>604</v>
+      <c r="F177" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="178">
@@ -25271,8 +25330,8 @@
       <c r="E178" s="0" t="n">
         <v>-0.13369718974012</v>
       </c>
-      <c r="F178" s="3" t="s">
-        <v>603</v>
+      <c r="F178" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="179">
@@ -25291,8 +25350,8 @@
       <c r="E179" s="0" t="n">
         <v>-0.1330938573102</v>
       </c>
-      <c r="F179" s="3" t="s">
-        <v>603</v>
+      <c r="F179" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="180">
@@ -25311,8 +25370,8 @@
       <c r="E180" s="0" t="n">
         <v>-0.38120935690424</v>
       </c>
-      <c r="F180" s="3" t="s">
-        <v>608</v>
+      <c r="F180" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="181">
@@ -25331,8 +25390,8 @@
       <c r="E181" s="0" t="n">
         <v>0.017795056275962</v>
       </c>
-      <c r="F181" s="3" t="s">
-        <v>602</v>
+      <c r="F181" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="182">
@@ -25351,8 +25410,8 @@
       <c r="E182" s="0" t="n">
         <v>-0.29495758553154</v>
       </c>
-      <c r="F182" s="3" t="s">
-        <v>604</v>
+      <c r="F182" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="183">
@@ -25371,8 +25430,8 @@
       <c r="E183" s="0" t="n">
         <v>-0.20935102262327</v>
       </c>
-      <c r="F183" s="3" t="s">
-        <v>607</v>
+      <c r="F183" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="184">
@@ -25391,8 +25450,8 @@
       <c r="E184" s="0" t="n">
         <v>-0.20478373421795</v>
       </c>
-      <c r="F184" s="3" t="s">
-        <v>607</v>
+      <c r="F184" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="185">
@@ -25411,8 +25470,8 @@
       <c r="E185" s="0" t="n">
         <v>-0.28631716346916</v>
       </c>
-      <c r="F185" s="3" t="s">
-        <v>604</v>
+      <c r="F185" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="186">
@@ -25431,8 +25490,8 @@
       <c r="E186" s="0" t="n">
         <v>-0.18740549543317</v>
       </c>
-      <c r="F186" s="3" t="s">
-        <v>603</v>
+      <c r="F186" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="187">
@@ -25451,8 +25510,8 @@
       <c r="E187" s="0" t="n">
         <v>-0.23595483065011</v>
       </c>
-      <c r="F187" s="3" t="s">
-        <v>607</v>
+      <c r="F187" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="188">
@@ -25471,8 +25530,8 @@
       <c r="E188" s="0" t="n">
         <v>-0.371046385824</v>
       </c>
-      <c r="F188" s="3" t="s">
-        <v>608</v>
+      <c r="F188" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="189">
@@ -25491,8 +25550,8 @@
       <c r="E189" s="0" t="n">
         <v>0.045408472505876</v>
       </c>
-      <c r="F189" s="3" t="s">
-        <v>604</v>
+      <c r="F189" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="190">
@@ -25511,8 +25570,8 @@
       <c r="E190" s="0" t="n">
         <v>-0.14532999904559</v>
       </c>
-      <c r="F190" s="3" t="s">
-        <v>603</v>
+      <c r="F190" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="191">
@@ -25531,8 +25590,8 @@
       <c r="E191" s="0" t="n">
         <v>-0.30172474133933</v>
       </c>
-      <c r="F191" s="3" t="s">
-        <v>604</v>
+      <c r="F191" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="192">
@@ -25551,8 +25610,8 @@
       <c r="E192" s="0" t="n">
         <v>-0.47367013575456</v>
       </c>
-      <c r="F192" s="3" t="s">
-        <v>611</v>
+      <c r="F192" s="2" t="s">
+        <v>614</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="193">
@@ -25571,8 +25630,8 @@
       <c r="E193" s="0" t="n">
         <v>0.044040648415103</v>
       </c>
-      <c r="F193" s="3" t="s">
-        <v>604</v>
+      <c r="F193" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="194">
@@ -25591,8 +25650,8 @@
       <c r="E194" s="0" t="n">
         <v>-0.18880926348942</v>
       </c>
-      <c r="F194" s="3" t="s">
-        <v>607</v>
+      <c r="F194" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="195">
@@ -25611,8 +25670,8 @@
       <c r="E195" s="0" t="n">
         <v>-0.42122049909957</v>
       </c>
-      <c r="F195" s="3" t="s">
-        <v>612</v>
+      <c r="F195" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="196">
@@ -25631,8 +25690,8 @@
       <c r="E196" s="0" t="n">
         <v>-0.40927968814014</v>
       </c>
-      <c r="F196" s="3" t="s">
-        <v>608</v>
+      <c r="F196" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="197">
@@ -25651,8 +25710,8 @@
       <c r="E197" s="0" t="n">
         <v>-0.41283492710738</v>
       </c>
-      <c r="F197" s="3" t="s">
-        <v>612</v>
+      <c r="F197" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="198">
@@ -25671,8 +25730,8 @@
       <c r="E198" s="0" t="n">
         <v>-0.12457578611157</v>
       </c>
-      <c r="F198" s="3" t="s">
-        <v>603</v>
+      <c r="F198" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="199">
@@ -25691,8 +25750,8 @@
       <c r="E199" s="0" t="n">
         <v>-0.0724523920649</v>
       </c>
-      <c r="F199" s="3" t="s">
-        <v>602</v>
+      <c r="F199" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="200">
@@ -25711,8 +25770,8 @@
       <c r="E200" s="0" t="n">
         <v>-0.21850475368199</v>
       </c>
-      <c r="F200" s="3" t="s">
-        <v>607</v>
+      <c r="F200" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="201">
@@ -25731,8 +25790,8 @@
       <c r="E201" s="0" t="n">
         <v>-0.22738608723774</v>
       </c>
-      <c r="F201" s="3" t="s">
-        <v>607</v>
+      <c r="F201" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="202">
@@ -25751,8 +25810,8 @@
       <c r="E202" s="0" t="n">
         <v>-0.1564744555002</v>
       </c>
-      <c r="F202" s="3" t="s">
-        <v>603</v>
+      <c r="F202" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="203">
@@ -25771,8 +25830,8 @@
       <c r="E203" s="0" t="n">
         <v>0.021478357761873</v>
       </c>
-      <c r="F203" s="3" t="s">
-        <v>604</v>
+      <c r="F203" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="204">
@@ -25791,8 +25850,8 @@
       <c r="E204" s="0" t="n">
         <v>-0.30702584019952</v>
       </c>
-      <c r="F204" s="3" t="s">
-        <v>602</v>
+      <c r="F204" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="205">
@@ -25811,8 +25870,8 @@
       <c r="E205" s="0" t="n">
         <v>-0.17390862058942</v>
       </c>
-      <c r="F205" s="3" t="s">
-        <v>603</v>
+      <c r="F205" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="206">
@@ -25831,8 +25890,8 @@
       <c r="E206" s="0" t="n">
         <v>-0.30812855062663</v>
       </c>
-      <c r="F206" s="3" t="s">
-        <v>604</v>
+      <c r="F206" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="207">
@@ -25851,8 +25910,8 @@
       <c r="E207" s="0" t="n">
         <v>-0.39910148824501</v>
       </c>
-      <c r="F207" s="3" t="s">
-        <v>608</v>
+      <c r="F207" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="208">
@@ -25871,11 +25930,11 @@
       <c r="E208" s="0" t="n">
         <v>-0.19196016848772</v>
       </c>
-      <c r="F208" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="G208" s="3" t="s">
-        <v>609</v>
+      <c r="F208" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="G208" s="2" t="s">
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="209">
@@ -25894,8 +25953,8 @@
       <c r="E209" s="0" t="n">
         <v>0.027957511681624</v>
       </c>
-      <c r="F209" s="3" t="s">
-        <v>604</v>
+      <c r="F209" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="210">
@@ -25914,8 +25973,8 @@
       <c r="E210" s="0" t="n">
         <v>-0.20659499856664</v>
       </c>
-      <c r="F210" s="3" t="s">
-        <v>602</v>
+      <c r="F210" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="211">
@@ -25934,8 +25993,8 @@
       <c r="E211" s="0" t="n">
         <v>-0.12775560097809</v>
       </c>
-      <c r="F211" s="3" t="s">
-        <v>604</v>
+      <c r="F211" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="212">
@@ -25954,8 +26013,8 @@
       <c r="E212" s="0" t="n">
         <v>-0.10578053394541</v>
       </c>
-      <c r="F212" s="3" t="s">
-        <v>603</v>
+      <c r="F212" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="213">
@@ -25974,8 +26033,8 @@
       <c r="E213" s="0" t="n">
         <v>-0.13386435110426</v>
       </c>
-      <c r="F213" s="3" t="s">
-        <v>603</v>
+      <c r="F213" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="214">
@@ -25994,8 +26053,8 @@
       <c r="E214" s="0" t="n">
         <v>-0.17405042505482</v>
       </c>
-      <c r="F214" s="3" t="s">
-        <v>607</v>
+      <c r="F214" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="215">
@@ -26014,8 +26073,8 @@
       <c r="E215" s="0" t="n">
         <v>-0.097556591574387</v>
       </c>
-      <c r="F215" s="3" t="s">
-        <v>603</v>
+      <c r="F215" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="216">
@@ -26034,8 +26093,8 @@
       <c r="E216" s="0" t="n">
         <v>-0.24523190696758</v>
       </c>
-      <c r="F216" s="3" t="s">
-        <v>607</v>
+      <c r="F216" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="217">
@@ -26054,8 +26113,8 @@
       <c r="E217" s="0" t="n">
         <v>-0.30308485086488</v>
       </c>
-      <c r="F217" s="3" t="s">
-        <v>608</v>
+      <c r="F217" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="218">
@@ -26074,8 +26133,8 @@
       <c r="E218" s="0" t="n">
         <v>-0.047368111957746</v>
       </c>
-      <c r="F218" s="3" t="s">
-        <v>607</v>
+      <c r="F218" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="219">
@@ -26094,8 +26153,8 @@
       <c r="E219" s="0" t="n">
         <v>-0.12283190859196</v>
       </c>
-      <c r="F219" s="3" t="s">
-        <v>607</v>
+      <c r="F219" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="220">
@@ -26114,8 +26173,8 @@
       <c r="E220" s="0" t="n">
         <v>-0.27538602336732</v>
       </c>
-      <c r="F220" s="3" t="s">
-        <v>602</v>
+      <c r="F220" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="221">
@@ -26134,8 +26193,8 @@
       <c r="E221" s="0" t="n">
         <v>-0.0037372234417709</v>
       </c>
-      <c r="F221" s="3" t="s">
-        <v>602</v>
+      <c r="F221" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="222">
@@ -26154,8 +26213,8 @@
       <c r="E222" s="0" t="n">
         <v>-0.33637769283987</v>
       </c>
-      <c r="F222" s="3" t="s">
-        <v>604</v>
+      <c r="F222" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="223">
@@ -26174,8 +26233,8 @@
       <c r="E223" s="0" t="n">
         <v>-0.31632906529511</v>
       </c>
-      <c r="F223" s="3" t="s">
-        <v>604</v>
+      <c r="F223" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="224">
@@ -26194,8 +26253,8 @@
       <c r="E224" s="0" t="n">
         <v>-0.17561218648329</v>
       </c>
-      <c r="F224" s="3" t="s">
-        <v>607</v>
+      <c r="F224" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="225">
@@ -26214,8 +26273,8 @@
       <c r="E225" s="0" t="n">
         <v>-0.11371134239066</v>
       </c>
-      <c r="F225" s="3" t="s">
-        <v>603</v>
+      <c r="F225" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="226">
@@ -26234,8 +26293,8 @@
       <c r="E226" s="0" t="n">
         <v>0.10290519530392</v>
       </c>
-      <c r="F226" s="3" t="s">
-        <v>612</v>
+      <c r="F226" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="227">
@@ -26254,8 +26313,8 @@
       <c r="E227" s="0" t="n">
         <v>-0.15968610811001</v>
       </c>
-      <c r="F227" s="3" t="s">
-        <v>602</v>
+      <c r="F227" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="228">
@@ -26274,8 +26333,8 @@
       <c r="E228" s="0" t="n">
         <v>-0.16867014599257</v>
       </c>
-      <c r="F228" s="3" t="s">
-        <v>602</v>
+      <c r="F228" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="229">
@@ -26294,8 +26353,8 @@
       <c r="E229" s="0" t="n">
         <v>-0.13109602942553</v>
       </c>
-      <c r="F229" s="3" t="s">
-        <v>603</v>
+      <c r="F229" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="230">
@@ -26314,8 +26373,8 @@
       <c r="E230" s="0" t="n">
         <v>-0.060173390466137</v>
       </c>
-      <c r="F230" s="3" t="s">
-        <v>602</v>
+      <c r="F230" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="231">
@@ -26334,8 +26393,8 @@
       <c r="E231" s="0" t="n">
         <v>-0.17933981753571</v>
       </c>
-      <c r="F231" s="3" t="s">
-        <v>604</v>
+      <c r="F231" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="232">
@@ -26354,8 +26413,8 @@
       <c r="E232" s="0" t="n">
         <v>-0.076686790760475</v>
       </c>
-      <c r="F232" s="3" t="s">
-        <v>603</v>
+      <c r="F232" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="233">
@@ -26374,8 +26433,8 @@
       <c r="E233" s="0" t="n">
         <v>-0.13772775294192</v>
       </c>
-      <c r="F233" s="3" t="s">
-        <v>607</v>
+      <c r="F233" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="234">
@@ -26394,8 +26453,8 @@
       <c r="E234" s="0" t="n">
         <v>-0.25451016527384</v>
       </c>
-      <c r="F234" s="3" t="s">
-        <v>607</v>
+      <c r="F234" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="235">
@@ -26414,8 +26473,8 @@
       <c r="E235" s="0" t="n">
         <v>-0.1027906082273</v>
       </c>
-      <c r="F235" s="3" t="s">
-        <v>602</v>
+      <c r="F235" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="236">
@@ -26434,8 +26493,8 @@
       <c r="E236" s="0" t="n">
         <v>0.2514152239117</v>
       </c>
-      <c r="F236" s="3" t="s">
-        <v>612</v>
+      <c r="F236" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="237">
@@ -26454,8 +26513,8 @@
       <c r="E237" s="0" t="n">
         <v>0.23455631120919</v>
       </c>
-      <c r="F237" s="3" t="s">
-        <v>612</v>
+      <c r="F237" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="238">
@@ -26474,8 +26533,8 @@
       <c r="E238" s="0" t="n">
         <v>0.10154616057314</v>
       </c>
-      <c r="F238" s="3" t="s">
-        <v>604</v>
+      <c r="F238" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="239">
@@ -26494,8 +26553,8 @@
       <c r="E239" s="0" t="n">
         <v>0.034556255633226</v>
       </c>
-      <c r="F239" s="3" t="s">
-        <v>602</v>
+      <c r="F239" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="240">
@@ -26514,8 +26573,8 @@
       <c r="E240" s="0" t="n">
         <v>-0.47708714109832</v>
       </c>
-      <c r="F240" s="3" t="s">
-        <v>612</v>
+      <c r="F240" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="241">
@@ -26534,11 +26593,11 @@
       <c r="E241" s="0" t="n">
         <v>-0.12381555294752</v>
       </c>
-      <c r="F241" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="G241" s="3" t="s">
-        <v>613</v>
+      <c r="F241" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="G241" s="2" t="s">
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="242">
@@ -26557,8 +26616,8 @@
       <c r="E242" s="0" t="n">
         <v>-0.14390630306143</v>
       </c>
-      <c r="F242" s="3" t="s">
-        <v>603</v>
+      <c r="F242" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="243">
@@ -26577,8 +26636,8 @@
       <c r="E243" s="0" t="n">
         <v>-0.019926114372123</v>
       </c>
-      <c r="F243" s="3" t="s">
-        <v>602</v>
+      <c r="F243" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="244">
@@ -26597,8 +26656,8 @@
       <c r="E244" s="0" t="n">
         <v>0.028774900468403</v>
       </c>
-      <c r="F244" s="3" t="s">
-        <v>604</v>
+      <c r="F244" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="245">
@@ -26617,8 +26676,8 @@
       <c r="E245" s="0" t="n">
         <v>-0.13826391949985</v>
       </c>
-      <c r="F245" s="3" t="s">
-        <v>603</v>
+      <c r="F245" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="246">
@@ -26637,8 +26696,8 @@
       <c r="E246" s="0" t="n">
         <v>-0.18293888140664</v>
       </c>
-      <c r="F246" s="3" t="s">
-        <v>607</v>
+      <c r="F246" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="247">
@@ -26657,8 +26716,8 @@
       <c r="E247" s="0" t="n">
         <v>-0.11324484659974</v>
       </c>
-      <c r="F247" s="3" t="s">
-        <v>603</v>
+      <c r="F247" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="248">
@@ -26677,8 +26736,8 @@
       <c r="E248" s="0" t="n">
         <v>-0.41725555293253</v>
       </c>
-      <c r="F248" s="3" t="s">
-        <v>611</v>
+      <c r="F248" s="2" t="s">
+        <v>614</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="249">
@@ -26697,8 +26756,8 @@
       <c r="E249" s="0" t="n">
         <v>-0.29637790641578</v>
       </c>
-      <c r="F249" s="3" t="s">
-        <v>604</v>
+      <c r="F249" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="250">
@@ -26717,8 +26776,8 @@
       <c r="E250" s="0" t="n">
         <v>-0.27922812839087</v>
       </c>
-      <c r="F250" s="3" t="s">
-        <v>604</v>
+      <c r="F250" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="251">
@@ -26737,8 +26796,8 @@
       <c r="E251" s="0" t="n">
         <v>-0.28064276561988</v>
       </c>
-      <c r="F251" s="3" t="s">
-        <v>602</v>
+      <c r="F251" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="252">
@@ -26757,8 +26816,8 @@
       <c r="E252" s="0" t="n">
         <v>-0.19552441152812</v>
       </c>
-      <c r="F252" s="3" t="s">
-        <v>607</v>
+      <c r="F252" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="253">
@@ -26777,8 +26836,8 @@
       <c r="E253" s="0" t="n">
         <v>-0.1889026706526</v>
       </c>
-      <c r="F253" s="3" t="s">
-        <v>604</v>
+      <c r="F253" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="254">
@@ -26797,8 +26856,8 @@
       <c r="E254" s="0" t="n">
         <v>0.0053318072586749</v>
       </c>
-      <c r="F254" s="3" t="s">
-        <v>602</v>
+      <c r="F254" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="255">
@@ -26817,8 +26876,8 @@
       <c r="E255" s="0" t="n">
         <v>-0.19111216622603</v>
       </c>
-      <c r="F255" s="3" t="s">
-        <v>607</v>
+      <c r="F255" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="256">
@@ -26837,8 +26896,8 @@
       <c r="E256" s="0" t="n">
         <v>-0.35383226807134</v>
       </c>
-      <c r="F256" s="3" t="s">
-        <v>608</v>
+      <c r="F256" s="2" t="s">
+        <v>612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="257">
@@ -26857,8 +26916,8 @@
       <c r="E257" s="0" t="n">
         <v>-0.20618929345907</v>
       </c>
-      <c r="F257" s="3" t="s">
-        <v>607</v>
+      <c r="F257" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="258">
@@ -26877,8 +26936,8 @@
       <c r="E258" s="0" t="n">
         <v>-0.43784571956141</v>
       </c>
-      <c r="F258" s="3" t="s">
-        <v>612</v>
+      <c r="F258" s="2" t="s">
+        <v>615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="259">
@@ -26897,8 +26956,8 @@
       <c r="E259" s="0" t="n">
         <v>-0.20086810419124</v>
       </c>
-      <c r="F259" s="3" t="s">
-        <v>607</v>
+      <c r="F259" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="260">
@@ -26917,8 +26976,8 @@
       <c r="E260" s="0" t="n">
         <v>-0.12498767440679</v>
       </c>
-      <c r="F260" s="3" t="s">
-        <v>603</v>
+      <c r="F260" s="2" t="s">
+        <v>608</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="261">
@@ -26937,8 +26996,8 @@
       <c r="E261" s="0" t="n">
         <v>-0.22461752326457</v>
       </c>
-      <c r="F261" s="3" t="s">
-        <v>607</v>
+      <c r="F261" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="262">
@@ -26957,8 +27016,8 @@
       <c r="E262" s="0" t="n">
         <v>-0.059406074587337</v>
       </c>
-      <c r="F262" s="3" t="s">
-        <v>607</v>
+      <c r="F262" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="263">
@@ -26977,8 +27036,8 @@
       <c r="E263" s="0" t="n">
         <v>-0.059406074587337</v>
       </c>
-      <c r="F263" s="3" t="s">
-        <v>607</v>
+      <c r="F263" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="264">
@@ -26997,11 +27056,11 @@
       <c r="E264" s="0" t="n">
         <v>-0.22239318421442</v>
       </c>
-      <c r="F264" s="3" t="s">
-        <v>606</v>
-      </c>
-      <c r="G264" s="3" t="s">
-        <v>606</v>
+      <c r="F264" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="G264" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="265">
@@ -27020,8 +27079,8 @@
       <c r="E265" s="0" t="n">
         <v>-0.2438947288224</v>
       </c>
-      <c r="F265" s="3" t="s">
-        <v>602</v>
+      <c r="F265" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="266">
@@ -27040,8 +27099,8 @@
       <c r="E266" s="0" t="n">
         <v>-0.20664845638008</v>
       </c>
-      <c r="F266" s="3" t="s">
-        <v>602</v>
+      <c r="F266" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="267">
@@ -27060,8 +27119,8 @@
       <c r="E267" s="0" t="n">
         <v>-0.19917189150183</v>
       </c>
-      <c r="F267" s="3" t="s">
-        <v>602</v>
+      <c r="F267" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="268">
@@ -27080,8 +27139,8 @@
       <c r="E268" s="0" t="n">
         <v>-0.10951215426353</v>
       </c>
-      <c r="F268" s="3" t="s">
-        <v>602</v>
+      <c r="F268" s="2" t="s">
+        <v>607</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="269">
@@ -27100,8 +27159,8 @@
       <c r="E269" s="0" t="n">
         <v>-0.2244582012666</v>
       </c>
-      <c r="F269" s="3" t="s">
-        <v>607</v>
+      <c r="F269" s="2" t="s">
+        <v>611</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="270">
@@ -27120,8 +27179,8 @@
       <c r="E270" s="0" t="n">
         <v>0.034070640659794</v>
       </c>
-      <c r="F270" s="3" t="s">
-        <v>604</v>
+      <c r="F270" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="271">
@@ -27140,8 +27199,8 @@
       <c r="E271" s="0" t="n">
         <v>-0.185411063095</v>
       </c>
-      <c r="F271" s="3" t="s">
-        <v>604</v>
+      <c r="F271" s="2" t="s">
+        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -27164,7 +27223,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="F5" activeCellId="0" pane="topLeft" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27252,7 +27311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
@@ -27269,7 +27328,7 @@
         <v>-0.10072431173602</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>14</v>
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
@@ -27712,7 +27771,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H9" activeCellId="0" pane="topLeft" sqref="H9"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28160,7 +28219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>330</v>
       </c>
@@ -28177,7 +28236,7 @@
         <v>0.009154878018083</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>90</v>
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
@@ -28280,7 +28339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
         <v>374</v>
       </c>
@@ -28296,8 +28355,8 @@
       <c r="E29" s="0" t="n">
         <v>-0.25971511616691</v>
       </c>
-      <c r="F29" s="0" t="s">
-        <v>99</v>
+      <c r="F29" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
@@ -28337,7 +28396,7 @@
         <v>-0.1959072111467</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>14</v>
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
@@ -28738,8 +28797,8 @@
   </sheetPr>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F24" activeCellId="0" pane="topLeft" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29224,7 +29283,7 @@
         <v>-0.1959072111467</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>14</v>
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
@@ -29485,8 +29544,8 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A32" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A29" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F69" activeCellId="0" pane="topLeft" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29694,7 +29753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>98</v>
       </c>
@@ -29710,8 +29769,8 @@
       <c r="E11" s="0" t="n">
         <v>-0.01166796209473</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>99</v>
+      <c r="F11" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
@@ -29851,7 +29910,7 @@
         <v>-0.19429940765557</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>14</v>
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
@@ -29871,10 +29930,10 @@
         <v>0.051530710126145</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
+        <v>603</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>187</v>
       </c>
@@ -29890,8 +29949,8 @@
       <c r="E20" s="0" t="n">
         <v>-0.21098384278422</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>99</v>
+      <c r="F20" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
@@ -30111,7 +30170,7 @@
         <v>-0.28536661446493</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>90</v>
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
@@ -30171,7 +30230,7 @@
         <v>-0.1959072111467</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>14</v>
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
@@ -30733,7 +30792,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="F9" activeCellId="0" pane="topLeft" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30861,7 +30920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>98</v>
       </c>
@@ -30877,8 +30936,8 @@
       <c r="E7" s="0" t="n">
         <v>-0.01166796209473</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>99</v>
+      <c r="F7" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
@@ -30898,7 +30957,7 @@
         <v>0.051530710126145</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>90</v>
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
@@ -31360,7 +31419,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="F16" activeCellId="0" pane="topLeft" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31668,7 +31727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>377</v>
       </c>
@@ -31684,8 +31743,8 @@
       <c r="E16" s="0" t="n">
         <v>0.0036006636371896</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>99</v>
+      <c r="F16" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
@@ -31908,7 +31967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>587</v>
       </c>
@@ -31924,8 +31983,8 @@
       <c r="E28" s="0" t="n">
         <v>-0.22239318421442</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>99</v>
+      <c r="F28" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -31946,8 +32005,8 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A5" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K29" activeCellId="0" pane="topLeft" sqref="K29"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F21" activeCellId="0" pane="topLeft" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32335,7 +32394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>353</v>
       </c>
@@ -32351,8 +32410,8 @@
       <c r="E20" s="0" t="n">
         <v>-0.4328985822977</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>354</v>
+      <c r="F20" s="2" t="s">
+        <v>605</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
@@ -32633,8 +32692,8 @@
   </sheetPr>
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G3" activeCellId="0" pane="topLeft" sqref="G3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A14" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F54" activeCellId="0" pane="topLeft" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32698,8 +32757,8 @@
       <c r="E3" s="0" t="n">
         <v>-0.13510715160572</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>41335</v>
+      <c r="F3" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
@@ -32921,9 +32980,9 @@
       <c r="F14" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K14" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
+      <c r="K14" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>144</v>
       </c>
@@ -32939,8 +32998,8 @@
       <c r="E15" s="0" t="n">
         <v>-0.1479696801021</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>99</v>
+      <c r="F15" s="2" t="s">
+        <v>604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
@@ -33040,7 +33099,7 @@
         <v>-0.10072431173602</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>14</v>
+        <v>602</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
@@ -33180,7 +33239,7 @@
         <v>-0.2267197095034</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>90</v>
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
@@ -33459,8 +33518,8 @@
       <c r="E41" s="0" t="n">
         <v>-0.19196016848772</v>
       </c>
-      <c r="F41" s="1" t="n">
-        <v>41367</v>
+      <c r="F41" s="1" t="s">
+        <v>603</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="42">

</xml_diff>